<commit_message>
z_ prefix to ignore
</commit_message>
<xml_diff>
--- a/01_Linear/Nachtfliegen_02.xlsx
+++ b/01_Linear/Nachtfliegen_02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bnr01a/Documents/data/ACU/20S/20S-MS/MSGit/01_Linear/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32726C06-485B-D449-A330-0F0ED66EDCB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A41B8EB-B31E-CD4A-BAC4-2FE9642ED7C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2520" windowWidth="27640" windowHeight="16940" activeTab="7" xr2:uid="{A7FC1D30-F79D-BE4F-B04A-26AC788931EB}"/>
+    <workbookView xWindow="3820" yWindow="4060" windowWidth="27640" windowHeight="16940" activeTab="7" xr2:uid="{A7FC1D30-F79D-BE4F-B04A-26AC788931EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -1896,7 +1896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8316985-0DCE-E34E-ACEB-D3AA3AB3F36C}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>